<commit_message>
last stuff from paper
</commit_message>
<xml_diff>
--- a/decode_dir/DailyDialog/metrics.xlsx
+++ b/decode_dir/DailyDialog/metrics.xlsx
@@ -1,16 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ricsi\GitHub\Seq2seqChatbots\decode_dir\DailyDialog\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C70E405-8624-4329-A7F3-D24C8871772E}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="7710" windowWidth="29040" windowHeight="15840" firstSheet="1" activeTab="7" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-28920" yWindow="7710" windowWidth="29040" windowHeight="15840" firstSheet="2" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="source_based_avg_embedding" sheetId="1" r:id="rId1"/>
@@ -41,8 +40,8 @@
 </file>
 
 <file path=xl/connections.xml><?xml version="1.0" encoding="utf-8"?>
-<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16">
-  <connection id="1" xr16:uid="{00000000-0015-0000-FFFF-FFFF00000000}" name="all_metrics" type="6" refreshedVersion="6" background="1" saveData="1">
+<connections xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <connection id="1" name="all_metrics" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="852" sourceFile="C:\Users\ricsi\GitHub\Seq2seqChatbots\decode_dir\DailyDialog\trf_20_dropout-base_source_based_avg_embedding\dev_metrics\all_metrics.txt" decimal="," thousands=" " tab="0" space="1" consecutive="1">
       <textFields count="16">
         <textField/>
@@ -64,7 +63,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="2" xr16:uid="{00000000-0015-0000-FFFF-FFFF01000000}" name="all_metrics1" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="2" name="all_metrics1" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="852" sourceFile="C:\Users\ricsi\GitHub\Seq2seqChatbots\decode_dir\DailyDialog\trf_20_dropout-base_both_sent_eval\dev_metrics\all_metrics.txt" decimal="," thousands=" " tab="0" space="1" consecutive="1">
       <textFields count="16">
         <textField/>
@@ -86,7 +85,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="3" xr16:uid="{00000000-0015-0000-FFFF-FFFF02000000}" name="all_metrics2" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="3" name="all_metrics2" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="852" sourceFile="C:\Users\ricsi\GitHub\Seq2seqChatbots\decode_dir\DailyDialog\trf_20_dropout-base_both_sent_eval\dev_metrics\all_metrics.txt" decimal="," thousands=" " tab="0" space="1" consecutive="1">
       <textFields count="16">
         <textField/>
@@ -108,7 +107,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="4" xr16:uid="{00000000-0015-0000-FFFF-FFFF03000000}" name="all_metrics3" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="4" name="all_metrics3" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="852" sourceFile="C:\Users\ricsi\GitHub\Seq2seqChatbots\decode_dir\DailyDialog\trf_20_dropout-base\dev_metrics\all_metrics.txt" decimal="," thousands=" " tab="0" space="1" consecutive="1">
       <textFields count="16">
         <textField/>
@@ -130,7 +129,7 @@
       </textFields>
     </textPr>
   </connection>
-  <connection id="5" xr16:uid="{D32AAE37-3336-467E-95F8-603C1310DB1E}" name="all_metrics4" type="6" refreshedVersion="6" background="1" saveData="1">
+  <connection id="5" name="all_metrics4" type="6" refreshedVersion="6" background="1" saveData="1">
     <textPr codePage="852" sourceFile="C:\Users\ricsi\GitHub\Seq2seqChatbots\decode_dir\DailyDialog\trf_20_dropout-base_with_numbers\dev_metrics\all_metrics.txt" decimal="," thousands=" " tab="0" space="1" consecutive="1">
       <textFields count="31">
         <textField/>
@@ -171,7 +170,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -7620,6 +7619,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -7627,7 +7627,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -7676,62 +7675,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="hu-HU"/>
-              <a:t>Distinct metrics of responses</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="hu-HU"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -8273,7 +8217,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -8292,6 +8236,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8305,7 +8250,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -8343,7 +8288,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -8362,6 +8307,39 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20000"/>
+        <c:dispUnits>
+          <c:builtInUnit val="thousands"/>
+          <c:dispUnitsLbl>
+            <c:layout/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="hu-HU"/>
+              </a:p>
+            </c:txPr>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
       </c:valAx>
       <c:valAx>
         <c:axId val="801541896"/>
@@ -8391,7 +8369,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -8410,6 +8388,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -8423,7 +8402,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -8461,7 +8440,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -8490,6 +8469,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8503,7 +8483,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -8521,6 +8501,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -8528,7 +8509,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -8550,7 +8530,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1800"/>
       </a:pPr>
       <a:endParaRPr lang="hu-HU"/>
     </a:p>
@@ -8577,62 +8557,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="hu-HU"/>
-              <a:t>Lengths of responses</a:t>
-            </a:r>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="hu-HU"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -9166,7 +9091,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -9180,16 +9105,12 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="hu-HU"/>
-                  <a:t>Training</a:t>
+                  <a:t>Training steps</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="hu-HU" baseline="0"/>
-                  <a:t> steps</a:t>
-                </a:r>
-                <a:endParaRPr lang="hu-HU"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9203,7 +9124,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -9241,7 +9162,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -9260,6 +9181,39 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20000"/>
+        <c:dispUnits>
+          <c:builtInUnit val="thousands"/>
+          <c:dispUnitsLbl>
+            <c:layout/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="hu-HU"/>
+              </a:p>
+            </c:txPr>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
       </c:valAx>
       <c:valAx>
         <c:axId val="638934696"/>
@@ -9290,7 +9244,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -9309,6 +9263,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -9322,7 +9277,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -9360,7 +9315,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -9389,6 +9344,7 @@
     </c:plotArea>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -9396,7 +9352,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -9418,7 +9373,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1800"/>
       </a:pPr>
       <a:endParaRPr lang="hu-HU"/>
     </a:p>
@@ -9445,75 +9400,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="hu-HU"/>
-              <a:t>Unigram</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="hu-HU" baseline="0"/>
-              <a:t> and bigram</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="hu-HU"/>
-              <a:t> entropy</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="hu-HU" baseline="0"/>
-              <a:t> of responses</a:t>
-            </a:r>
-            <a:endParaRPr lang="hu-HU"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="hu-HU"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -10541,7 +10428,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -10560,6 +10447,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -10573,7 +10461,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -10611,7 +10499,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -10630,6 +10518,39 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20000"/>
+        <c:dispUnits>
+          <c:builtInUnit val="thousands"/>
+          <c:dispUnitsLbl>
+            <c:layout/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="hu-HU"/>
+              </a:p>
+            </c:txPr>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
       </c:valAx>
       <c:valAx>
         <c:axId val="632312552"/>
@@ -10660,7 +10581,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -10679,6 +10600,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -10692,7 +10614,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -10730,7 +10652,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -10759,6 +10681,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -10772,7 +10695,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -10790,6 +10713,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -10797,7 +10721,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -10819,7 +10742,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1800"/>
       </a:pPr>
       <a:endParaRPr lang="hu-HU"/>
     </a:p>
@@ -10846,75 +10769,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="hu-HU"/>
-              <a:t>Unigram and</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="hu-HU" baseline="0"/>
-              <a:t> bigram u</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="hu-HU"/>
-              <a:t>tterance entropy</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="hu-HU" baseline="0"/>
-              <a:t> of responses</a:t>
-            </a:r>
-            <a:endParaRPr lang="hu-HU"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="hu-HU"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -11942,7 +11797,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -11961,6 +11816,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -11974,7 +11830,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -12012,7 +11868,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -12031,6 +11887,39 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20000"/>
+        <c:dispUnits>
+          <c:builtInUnit val="thousands"/>
+          <c:dispUnitsLbl>
+            <c:layout/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="hu-HU"/>
+              </a:p>
+            </c:txPr>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
       </c:valAx>
       <c:valAx>
         <c:axId val="801567808"/>
@@ -12061,7 +11950,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -12080,6 +11969,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -12093,7 +11983,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -12131,7 +12021,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -12160,6 +12050,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12173,7 +12064,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -12191,6 +12082,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -12198,7 +12090,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -12220,7 +12111,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1800"/>
       </a:pPr>
       <a:endParaRPr lang="hu-HU"/>
     </a:p>
@@ -12247,67 +12138,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="hu-HU"/>
-              <a:t>Unigram</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="hu-HU" baseline="0"/>
-              <a:t> and bigram KL-divergences of responses and targets</a:t>
-            </a:r>
-            <a:endParaRPr lang="hu-HU"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="hu-HU"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -13335,7 +13166,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -13349,16 +13180,12 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="hu-HU"/>
-                  <a:t>Training</a:t>
+                  <a:t>Training steps</a:t>
                 </a:r>
-                <a:r>
-                  <a:rPr lang="hu-HU" baseline="0"/>
-                  <a:t> steps</a:t>
-                </a:r>
-                <a:endParaRPr lang="hu-HU"/>
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -13372,7 +13199,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -13410,7 +13237,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -13429,6 +13256,39 @@
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
         <c:majorUnit val="20000"/>
+        <c:dispUnits>
+          <c:builtInUnit val="thousands"/>
+          <c:dispUnitsLbl>
+            <c:layout/>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:txPr>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:endParaRPr lang="hu-HU"/>
+              </a:p>
+            </c:txPr>
+          </c:dispUnitsLbl>
+        </c:dispUnits>
       </c:valAx>
       <c:valAx>
         <c:axId val="801549112"/>
@@ -13458,7 +13318,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -13477,6 +13337,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -13490,7 +13351,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -13528,7 +13389,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -13557,6 +13418,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -13570,7 +13432,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -13588,6 +13450,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -13595,7 +13458,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -13617,7 +13479,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1800"/>
       </a:pPr>
       <a:endParaRPr lang="hu-HU"/>
     </a:p>
@@ -13644,67 +13506,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="hu-HU"/>
-              <a:t>Embedding</a:t>
-            </a:r>
-            <a:r>
-              <a:rPr lang="hu-HU" baseline="0"/>
-              <a:t> metrics of responses</a:t>
-            </a:r>
-            <a:endParaRPr lang="hu-HU"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="hu-HU"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:scatterChart>
@@ -13714,10 +13516,10 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Embedding average</c:v>
+            <c:v>Emb. Avg.</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="38100" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
@@ -14204,10 +14006,10 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:v>Embedding extrema</c:v>
+            <c:v>Emb. Ext.</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="38100" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
@@ -14695,10 +14497,10 @@
           <c:idx val="2"/>
           <c:order val="2"/>
           <c:tx>
-            <c:v>Embedding greedy</c:v>
+            <c:v>Emb. greedy</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="38100" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent3"/>
               </a:solidFill>
@@ -15186,10 +14988,10 @@
           <c:idx val="3"/>
           <c:order val="3"/>
           <c:tx>
-            <c:v>Cos. Sim. between response and input</c:v>
+            <c:v>Coherence</c:v>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="38100" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent4"/>
               </a:solidFill>
@@ -15688,7 +15490,7 @@
         <c:axId val="710329752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="310000"/>
+          <c:max val="140000"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -15714,7 +15516,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -15733,6 +15535,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -15746,7 +15549,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -15784,7 +15587,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -15808,7 +15611,8 @@
         <c:axId val="710329096"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:min val="0.4"/>
+          <c:max val="0.70000000000000007"/>
+          <c:min val="0.45"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="l"/>
@@ -15833,7 +15637,7 @@
               <a:lstStyle/>
               <a:p>
                 <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                     <a:solidFill>
                       <a:schemeClr val="tx1">
                         <a:lumMod val="65000"/>
@@ -15852,6 +15656,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -15865,7 +15670,7 @@
             <a:lstStyle/>
             <a:p>
               <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                   <a:solidFill>
                     <a:schemeClr val="tx1">
                       <a:lumMod val="65000"/>
@@ -15903,7 +15708,7 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
@@ -15932,6 +15737,7 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15945,7 +15751,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -15963,6 +15769,7 @@
     </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
     <c:extLst>
       <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
         <c16r3:dataDisplayOptions16>
@@ -15970,7 +15777,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
     <a:solidFill>
@@ -15992,7 +15798,7 @@
     <a:lstStyle/>
     <a:p>
       <a:pPr>
-        <a:defRPr/>
+        <a:defRPr sz="1800"/>
       </a:pPr>
       <a:endParaRPr lang="hu-HU"/>
     </a:p>
@@ -35380,15 +35186,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>1</xdr:colOff>
+      <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>542925</xdr:colOff>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>180975</xdr:colOff>
       <xdr:row>35</xdr:row>
-      <xdr:rowOff>28575</xdr:rowOff>
+      <xdr:rowOff>19051</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -35983,10 +35789,10 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>28576</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>133350</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>66674</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -36026,10 +35832,10 @@
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>17</xdr:col>
-      <xdr:colOff>390525</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>114300</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -36069,10 +35875,10 @@
       <xdr:rowOff>1</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>609600</xdr:colOff>
-      <xdr:row>35</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>323850</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -36109,13 +35915,13 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>18</xdr:col>
-      <xdr:colOff>466725</xdr:colOff>
-      <xdr:row>34</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>57150</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>38099</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -36155,8 +35961,8 @@
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>19</xdr:col>
-      <xdr:colOff>114300</xdr:colOff>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
@@ -36189,23 +35995,23 @@
 </file>
 
 <file path=xl/queryTables/queryTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="all_metrics" connectionId="1" xr16:uid="{00000000-0016-0000-0000-000000000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="all_metrics" connectionId="1" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="all_metrics_1" connectionId="3" xr16:uid="{00000000-0016-0000-0100-000001000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="all_metrics" connectionId="2" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="all_metrics" connectionId="2" xr16:uid="{00000000-0016-0000-0100-000002000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="all_metrics_1" connectionId="3" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="all_metrics" connectionId="4" xr16:uid="{00000000-0016-0000-0200-000003000000}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="all_metrics" connectionId="4" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/queryTables/queryTable5.xml><?xml version="1.0" encoding="utf-8"?>
-<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr16="http://schemas.microsoft.com/office/spreadsheetml/2017/revision16" mc:Ignorable="xr16" name="all_metrics_1" connectionId="5" xr16:uid="{90494468-F1B8-4703-81D1-4E941F69B64F}" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
+<queryTable xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" name="all_metrics_1" connectionId="5" autoFormatId="16" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="0"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -36470,26 +36276,26 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A2:P16"/>
   <sheetViews>
     <sheetView zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="S25" sqref="S25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="6" bestFit="1" customWidth="1"/>
-    <col min="2" max="6" width="18.84375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.84375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.84375" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="18.84375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.84375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.84375" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="18.84375" bestFit="1" customWidth="1"/>
+    <col min="2" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>30627</v>
       </c>
@@ -36539,7 +36345,7 @@
         <v>0.63686250521947696</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>33414</v>
       </c>
@@ -36589,7 +36395,7 @@
         <v>0.664369050847191</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>36202</v>
       </c>
@@ -36639,7 +36445,7 @@
         <v>0.70702240043332099</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>38991</v>
       </c>
@@ -36689,7 +36495,7 @@
         <v>0.72237239324722602</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>41779</v>
       </c>
@@ -36739,7 +36545,7 @@
         <v>0.70951770509758905</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>44566</v>
       </c>
@@ -36789,7 +36595,7 @@
         <v>0.72879277194738601</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>47352</v>
       </c>
@@ -36839,7 +36645,7 @@
         <v>0.75377762332613796</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>50139</v>
       </c>
@@ -36889,7 +36695,7 @@
         <v>0.74502064949714897</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>52925</v>
       </c>
@@ -36939,7 +36745,7 @@
         <v>0.77091031014820299</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>55711</v>
       </c>
@@ -36989,7 +36795,7 @@
         <v>0.778577475246921</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>58498</v>
       </c>
@@ -37039,7 +36845,7 @@
         <v>0.77993250694467398</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>61286</v>
       </c>
@@ -37089,7 +36895,7 @@
         <v>0.78670763381939401</v>
       </c>
     </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>64076</v>
       </c>
@@ -37139,7 +36945,7 @@
         <v>0.794456829448417</v>
       </c>
     </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>66865</v>
       </c>
@@ -37189,7 +36995,7 @@
         <v>0.77196087771500299</v>
       </c>
     </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>69653</v>
       </c>
@@ -37246,14 +37052,14 @@
 </file>
 
 <file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C3195D61-DFD2-4562-8882-C41DC2A48E36}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="O47" sqref="O47"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="W12" sqref="W12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -37261,28 +37067,28 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P13"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="N1" activeCellId="1" sqref="A1:A13 N1:N13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="7.3828125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="19.69140625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.69140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="6" width="19.69140625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.69140625" customWidth="1"/>
-    <col min="8" max="8" width="20.69140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="19.69140625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.69140625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="20.69140625" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="19.69140625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="7.42578125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="6" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.7109375" customWidth="1"/>
+    <col min="8" max="8" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.7109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="20.7109375" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="19.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>46641</v>
       </c>
@@ -37332,7 +37138,7 @@
         <v>0.73466218199442901</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>49102</v>
       </c>
@@ -37382,7 +37188,7 @@
         <v>0.75558456448914202</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>54026</v>
       </c>
@@ -37432,7 +37238,7 @@
         <v>0.79751729443447394</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>56485</v>
       </c>
@@ -37482,7 +37288,7 @@
         <v>0.78005909684474495</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>61407</v>
       </c>
@@ -37532,7 +37338,7 @@
         <v>0.77541268723727297</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>66329</v>
       </c>
@@ -37582,7 +37388,7 @@
         <v>0.77553578884936403</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>71246</v>
       </c>
@@ -37632,7 +37438,7 @@
         <v>0.78251828432419201</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>76172</v>
       </c>
@@ -37682,7 +37488,7 @@
         <v>0.80164082573433204</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>81096</v>
       </c>
@@ -37732,7 +37538,7 @@
         <v>0.78857378261813404</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>86030</v>
       </c>
@@ -37782,7 +37588,7 @@
         <v>0.78888400475356701</v>
       </c>
     </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>90959</v>
       </c>
@@ -37832,7 +37638,7 @@
         <v>0.79270329465683698</v>
       </c>
     </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>95888</v>
       </c>
@@ -37882,7 +37688,7 @@
         <v>0.78198059376299001</v>
       </c>
     </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>100000</v>
       </c>
@@ -37942,28 +37748,28 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P10"/>
   <sheetViews>
     <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
       <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="7" bestFit="1" customWidth="1"/>
-    <col min="2" max="4" width="18.84375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="17.84375" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.84375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.84375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="19.84375" bestFit="1" customWidth="1"/>
-    <col min="9" max="12" width="18.84375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.84375" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.84375" bestFit="1" customWidth="1"/>
-    <col min="15" max="16" width="18.84375" bestFit="1" customWidth="1"/>
+    <col min="2" max="4" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="17.85546875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="9" max="12" width="18.85546875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.85546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.85546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="18.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>22001</v>
       </c>
@@ -38013,7 +37819,7 @@
         <v>0.60754609198299703</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>33001</v>
       </c>
@@ -38063,7 +37869,7 @@
         <v>0.71668656839447997</v>
       </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>44001</v>
       </c>
@@ -38113,7 +37919,7 @@
         <v>0.79379894800860396</v>
       </c>
     </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>66001</v>
       </c>
@@ -38163,7 +37969,7 @@
         <v>0.818198583601774</v>
       </c>
     </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>88001</v>
       </c>
@@ -38213,7 +38019,7 @@
         <v>0.83184867545229102</v>
       </c>
     </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>109001</v>
       </c>
@@ -38263,7 +38069,7 @@
         <v>0.82351468432701802</v>
       </c>
     </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>142001</v>
       </c>
@@ -38313,7 +38119,7 @@
         <v>0.82652175235552205</v>
       </c>
     </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>175001</v>
       </c>
@@ -38363,7 +38169,7 @@
         <v>0.81637138835505696</v>
       </c>
     </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>218001</v>
       </c>
@@ -38413,7 +38219,7 @@
         <v>0.83301669606929196</v>
       </c>
     </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>225001</v>
       </c>
@@ -38473,45 +38279,45 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A44509A7-FD13-41DD-9824-0647A151B383}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AE32"/>
   <sheetViews>
     <sheetView topLeftCell="F1" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
       <selection activeCell="Z1" activeCellId="2" sqref="A1:A32 X1:X32 Z1:Z32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.84375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="18.53515625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.53515625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="18.53515625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="20.53515625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.53515625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="20.53515625" bestFit="1" customWidth="1"/>
-    <col min="8" max="11" width="18.53515625" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.53515625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="21.61328125" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.53515625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="21.61328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="19.53515625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="21.61328125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="19.53515625" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="21.61328125" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="18.53515625" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="21.61328125" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="19.53515625" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="21.61328125" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="3.3828125" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="20.53515625" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="3.3828125" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="20.53515625" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="3.3828125" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="19.53515625" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="3.3828125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="6.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="8" max="11" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="18.5703125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="21.5703125" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="20.5703125" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="3.42578125" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="19.5703125" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="3.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A1">
         <v>2402</v>
       </c>
@@ -38606,7 +38412,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>4875</v>
       </c>
@@ -38701,7 +38507,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>7344</v>
       </c>
@@ -38796,7 +38602,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>9808</v>
       </c>
@@ -38891,7 +38697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>12265</v>
       </c>
@@ -38986,7 +38792,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>14726</v>
       </c>
@@ -39081,7 +38887,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>17179</v>
       </c>
@@ -39176,7 +38982,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>19635</v>
       </c>
@@ -39271,7 +39077,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>22082</v>
       </c>
@@ -39366,7 +39172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>26998</v>
       </c>
@@ -39461,7 +39267,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="11" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>31904</v>
       </c>
@@ -39556,7 +39362,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>36822</v>
       </c>
@@ -39651,7 +39457,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>41741</v>
       </c>
@@ -39746,7 +39552,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>51563</v>
       </c>
@@ -39841,7 +39647,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>61415</v>
       </c>
@@ -39936,7 +39742,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>71275</v>
       </c>
@@ -40031,7 +39837,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>81097</v>
       </c>
@@ -40126,7 +39932,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>90920</v>
       </c>
@@ -40221,7 +40027,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>104981</v>
       </c>
@@ -40316,7 +40122,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="20" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>120235</v>
       </c>
@@ -40411,7 +40217,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>135572</v>
       </c>
@@ -40506,7 +40312,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>150918</v>
       </c>
@@ -40601,7 +40407,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>166277</v>
       </c>
@@ -40696,7 +40502,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>181743</v>
       </c>
@@ -40791,7 +40597,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>197231</v>
       </c>
@@ -40886,7 +40692,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="26" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>212863</v>
       </c>
@@ -40981,7 +40787,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="27" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>228509</v>
       </c>
@@ -41076,7 +40882,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>244148</v>
       </c>
@@ -41171,7 +40977,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>259787</v>
       </c>
@@ -41266,7 +41072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>275414</v>
       </c>
@@ -41361,7 +41167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>291016</v>
       </c>
@@ -41456,7 +41262,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:31" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:31" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>300000</v>
       </c>
@@ -41561,12 +41367,12 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8CFF468E-181B-4825-B6DA-6F7D32082FEF}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -41574,14 +41380,14 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EBC72C2-DFF4-41DF-BC33-5BE40CADC442}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="H47" sqref="H47"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -41589,12 +41395,12 @@
 </file>
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B5CC0C1-4621-4C55-9C4C-3C5DFDE4B277}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -41602,14 +41408,14 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{238228AC-7FC1-45BB-B778-6DC161D8513F}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="X22" sqref="X22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
@@ -41617,12 +41423,12 @@
 </file>
 
 <file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E547CA2F-B50B-43DA-9C9A-D665CA35B5C9}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>